<commit_message>
Thres update to multiple area abs sum
</commit_message>
<xml_diff>
--- a/config/OTFS.xlsx
+++ b/config/OTFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github_Textremo\Phy_Joint_VBPIC\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50699AB-3D61-4B22-B880-83F6AE71C334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E7163C-B7A9-40FF-BA55-DB926D190A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-72" yWindow="-13068" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>toy</t>
+  </si>
+  <si>
+    <t>otfs-sbl</t>
   </si>
 </sst>
 </file>
@@ -721,160 +724,211 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B055A9B-D1C9-4DCA-B7F0-389C12C15A8C}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="A16:B17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="3">
         <v>10000</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B16">
+        <v>63</v>
+      </c>
+      <c r="C16">
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B17">
+        <v>63</v>
+      </c>
+      <c r="C17">
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
     </row>
   </sheetData>

</xml_diff>